<commit_message>
Hyper links in readme
</commit_message>
<xml_diff>
--- a/Logboek/Logboek werkwijze.xlsx
+++ b/Logboek/Logboek werkwijze.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31613\Documents\Mediacollege Amsterdam\Leerjaar 2\Periode 2.2\Radicale kunstspeeltuin\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70761C69-BD44-4C1E-9DEC-0F8941B402B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5320903-E04C-4113-85CF-F5FC12DB66E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8E2B147-EA8F-468F-BA10-E1A0455F2466}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Waar</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>2/12/2021  09:00 - 15:45    (Sprint 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We hebben beslist dat we een app gaan maken waarmee je informatie op kan vinden en licht mee kan veranderen. </t>
   </si>
 </sst>
 </file>
@@ -328,6 +331,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -355,6 +385,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,51 +411,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,60 +729,60 @@
   <dimension ref="B2:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:W25"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="40"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="37"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="43"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -806,36 +809,36 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="29" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="29" t="s">
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="29" t="s">
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="31"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46"/>
     </row>
     <row r="6" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -848,26 +851,26 @@
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="39"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="20" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="22"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="31"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
@@ -876,22 +879,22 @@
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="25"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="34"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
@@ -900,22 +903,22 @@
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="25"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="34"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
@@ -924,22 +927,22 @@
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="28"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="37"/>
     </row>
     <row r="10" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -952,26 +955,26 @@
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="39"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="20" t="s">
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="22"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="31"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
@@ -980,22 +983,22 @@
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="25"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="34"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
@@ -1004,22 +1007,22 @@
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="25"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="34"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="8"/>
@@ -1028,22 +1031,22 @@
       <c r="E13" s="17"/>
       <c r="F13" s="18"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="28"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="37"/>
     </row>
     <row r="14" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -1056,26 +1059,26 @@
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="20" t="s">
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="22"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="31"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
@@ -1084,22 +1087,22 @@
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
       <c r="G15" s="16"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="25"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="34"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
@@ -1108,22 +1111,22 @@
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="25"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" s="8"/>
@@ -1132,22 +1135,22 @@
       <c r="E17" s="17"/>
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="28"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="37"/>
     </row>
     <row r="18" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
@@ -1160,26 +1163,26 @@
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="38" t="s">
+      <c r="H18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="20" t="s">
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="22"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="31"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
@@ -1188,22 +1191,22 @@
       <c r="E19" s="14"/>
       <c r="F19" s="15"/>
       <c r="G19" s="16"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="25"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="34"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
@@ -1212,22 +1215,22 @@
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="16"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="25"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="34"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21" s="8"/>
@@ -1236,22 +1239,22 @@
       <c r="E21" s="17"/>
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="28"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="37"/>
     </row>
     <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
@@ -1264,24 +1267,26 @@
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="38" t="s">
+      <c r="H22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="39"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="22"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="31"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
@@ -1290,22 +1295,22 @@
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
       <c r="G23" s="16"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="25"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="34"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
@@ -1314,22 +1319,22 @@
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="16"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="25"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="34"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B25" s="8"/>
@@ -1338,34 +1343,25 @@
       <c r="E25" s="17"/>
       <c r="F25" s="18"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="27"/>
-      <c r="W25" s="28"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="36"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B14:D17"/>
-    <mergeCell ref="E14:G17"/>
-    <mergeCell ref="H14:J17"/>
-    <mergeCell ref="K14:W17"/>
-    <mergeCell ref="B2:W3"/>
-    <mergeCell ref="B6:D9"/>
-    <mergeCell ref="E6:G9"/>
-    <mergeCell ref="H6:J9"/>
-    <mergeCell ref="K6:W9"/>
     <mergeCell ref="B22:D25"/>
     <mergeCell ref="E22:G25"/>
     <mergeCell ref="H22:J25"/>
@@ -1382,6 +1378,15 @@
     <mergeCell ref="H18:J21"/>
     <mergeCell ref="K18:W21"/>
     <mergeCell ref="K10:W13"/>
+    <mergeCell ref="B14:D17"/>
+    <mergeCell ref="E14:G17"/>
+    <mergeCell ref="H14:J17"/>
+    <mergeCell ref="K14:W17"/>
+    <mergeCell ref="B2:W3"/>
+    <mergeCell ref="B6:D9"/>
+    <mergeCell ref="E6:G9"/>
+    <mergeCell ref="H6:J9"/>
+    <mergeCell ref="K6:W9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>